<commit_message>
comprobado para tres números
</commit_message>
<xml_diff>
--- a/pilas/pasar3aB.xlsx
+++ b/pilas/pasar3aB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apa\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apa/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536030B3-AA0D-474F-8B4A-0BB0956C278A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCE24B3-3BAF-314A-8A18-FF7EBF4C463F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{88ABF38A-BBD6-4276-A244-19E092795D5F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12640" windowHeight="21600" xr2:uid="{88ABF38A-BBD6-4276-A244-19E092795D5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -98,6 +98,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -111,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -121,6 +127,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -139,7 +146,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -435,42 +442,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A2085F5-F5D2-4CD1-85F9-59E87D593D14}">
-  <dimension ref="C2:AC14"/>
+  <dimension ref="C2:Z14"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="3:29" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:26" x14ac:dyDescent="0.2">
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="R2" t="s">
+      <c r="O2" t="s">
         <v>7</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="3:29" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C3" s="1"/>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5">
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="3">
+      <c r="I3" s="3">
+        <v>3</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -479,108 +488,104 @@
       <c r="L3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="R3" s="3">
-        <v>3</v>
-      </c>
-      <c r="S3" s="3">
-        <v>2</v>
-      </c>
-      <c r="T3" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA3">
-        <v>3</v>
-      </c>
-      <c r="AB3">
-        <v>2</v>
-      </c>
-      <c r="AC3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="3:29" x14ac:dyDescent="0.35">
+      <c r="M3" s="1"/>
+      <c r="O3" s="3">
+        <v>3</v>
+      </c>
+      <c r="P3" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>1</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>3</v>
+      </c>
+      <c r="Y3">
+        <v>2</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C4" s="1"/>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5">
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="3">
-        <v>4</v>
+      <c r="I4" s="3">
+        <v>4</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O4" s="1"/>
-      <c r="R4" s="3">
-        <v>3</v>
-      </c>
-      <c r="S4" s="3">
-        <v>2</v>
-      </c>
-      <c r="T4" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA4">
-        <v>1</v>
-      </c>
-      <c r="AB4">
-        <v>3</v>
-      </c>
-      <c r="AC4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="3:29" x14ac:dyDescent="0.35">
+      <c r="O4" s="3">
+        <v>3</v>
+      </c>
+      <c r="P4" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>1</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>3</v>
+      </c>
+      <c r="Z4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C5" s="1"/>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
         <v>3</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="3">
+      <c r="I5" s="3">
+        <v>4</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>3</v>
@@ -588,49 +593,47 @@
       <c r="M5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O5" s="1"/>
-      <c r="R5" s="3">
-        <v>3</v>
-      </c>
-      <c r="S5" s="3">
-        <v>2</v>
-      </c>
-      <c r="T5" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA5">
-        <v>2</v>
-      </c>
-      <c r="AB5">
-        <v>1</v>
-      </c>
-      <c r="AC5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="3:29" x14ac:dyDescent="0.35">
+      <c r="O5" s="3">
+        <v>3</v>
+      </c>
+      <c r="P5" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>1</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>2</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C6" s="1"/>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
+      <c r="D6" s="5">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="4">
+      <c r="I6" s="4">
+        <v>3</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -639,38 +642,37 @@
       <c r="L6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N6" s="1"/>
-      <c r="R6" s="4">
-        <v>1</v>
-      </c>
-      <c r="S6" s="4">
-        <v>3</v>
-      </c>
-      <c r="T6" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="3:29" x14ac:dyDescent="0.35">
+      <c r="M6" s="1"/>
+      <c r="O6" s="4">
+        <v>1</v>
+      </c>
+      <c r="P6" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C7" s="1"/>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
+      <c r="D7" s="5">
+        <v>3</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
         <v>2</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="4">
-        <v>4</v>
+      <c r="I7" s="4">
+        <v>4</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>3</v>
@@ -678,41 +680,39 @@
       <c r="L7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="4">
-        <v>2</v>
-      </c>
-      <c r="S7" s="4">
-        <v>1</v>
-      </c>
-      <c r="T7" s="4">
-        <v>3</v>
-      </c>
-      <c r="U7" s="1"/>
-    </row>
-    <row r="8" spans="3:29" x14ac:dyDescent="0.35">
+      <c r="O7" s="4">
+        <v>2</v>
+      </c>
+      <c r="P7" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>3</v>
+      </c>
+      <c r="R7" s="1"/>
+    </row>
+    <row r="8" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C8" s="1"/>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
+      <c r="D8" s="5">
+        <v>3</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2</v>
+      </c>
+      <c r="F8" s="5">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="4">
-        <v>4</v>
+      <c r="I8" s="4">
+        <v>4</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>3</v>
@@ -721,38 +721,34 @@
         <v>3</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="R8" s="4">
-        <v>2</v>
-      </c>
-      <c r="S8" s="4">
-        <v>1</v>
-      </c>
-      <c r="T8" s="4">
-        <v>3</v>
-      </c>
+      <c r="O8" s="4">
+        <v>2</v>
+      </c>
+      <c r="P8" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>3</v>
+      </c>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-    </row>
-    <row r="9" spans="3:29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C9" s="1"/>
     </row>
-    <row r="13" spans="3:29" x14ac:dyDescent="0.35">
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="3:29" x14ac:dyDescent="0.35">
-      <c r="M14" s="1"/>
+    <row r="13" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="L14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -760,13 +756,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754C003B-A17D-4071-9E5C-796D3DB00163}">
   <dimension ref="C2:AD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:30" x14ac:dyDescent="0.2">
       <c r="D2" t="s">
         <v>8</v>
       </c>
@@ -777,7 +773,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C3" s="1"/>
       <c r="D3">
         <v>1</v>
@@ -835,7 +831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:30" x14ac:dyDescent="0.2">
       <c r="D4">
         <v>1</v>
       </c>
@@ -894,7 +890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:30" x14ac:dyDescent="0.2">
       <c r="D5">
         <v>1</v>
       </c>
@@ -923,7 +919,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:30" x14ac:dyDescent="0.2">
       <c r="D6">
         <v>1</v>
       </c>
@@ -952,7 +948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:30" x14ac:dyDescent="0.2">
       <c r="D7">
         <v>1</v>
       </c>
@@ -966,7 +962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:30" x14ac:dyDescent="0.2">
       <c r="D8">
         <v>1</v>
       </c>
@@ -980,7 +976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:30" x14ac:dyDescent="0.2">
       <c r="Q10" t="s">
         <v>0</v>
       </c>
@@ -997,7 +993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:30" x14ac:dyDescent="0.2">
       <c r="Q11" t="s">
         <v>1</v>
       </c>

</xml_diff>